<commit_message>
Updated with comments from Anatoly and David
</commit_message>
<xml_diff>
--- a/notes/My_BoM.xlsx
+++ b/notes/My_BoM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="183">
   <si>
     <t xml:space="preserve">Frame</t>
   </si>
@@ -67,16 +67,37 @@
     <t xml:space="preserve">Need these when tabs get in the way "20s 10pcs black"</t>
   </si>
   <si>
-    <t xml:space="preserve">Frame Kits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aluminum frame kit in 4 colors: Black/Blue/Red/Purple - anodized after cut+Brackets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sealand (Aliexp)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Black" "Full Frame Kit" comes with the hardware as well</t>
+    <t xml:space="preserve">Frame Kit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aluminum frame kit (365mm Z Height Standard Frame)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FYSETC (Aliexp)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">"Full Set Kit". </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">This isn’t actually the one I ordered but I believe it’s the same kit. Mine isn’t available any longer</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.aliexpress.com/item/33048238537.html?spm=a2g0o.productlist.0.0.3b59553bEb0n4Z&amp;algo_pvid=ee9d284c-5474-4a38-9f09-9532647a402f&amp;algo_expid=ee9d284c-5474-4a38-9f09-9532647a402f-2&amp;btsid=0b0a556216108909047922816e4e3b&amp;ws_ab_test=searchweb0_0,searchweb201602_,searchweb201603_</t>
   </si>
   <si>
     <t xml:space="preserve">Motion System</t>
@@ -575,12 +596,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -602,6 +624,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -609,9 +632,17 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -660,7 +691,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -674,6 +705,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -694,15 +733,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:AMJ158"/>
+  <dimension ref="A2:L158"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
+      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.48"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="1" width="14.43"/>
   </cols>
   <sheetData>
     <row r="2" s="2" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -782,7 +822,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -809,8 +849,11 @@
       <c r="I7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="4" t="s">
         <v>18</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -821,12 +864,12 @@
     </row>
     <row r="9" s="2" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F10" s="1" t="n">
         <f aca="false">SUM(C10:E10)</f>
@@ -835,7 +878,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="n">
         <f aca="false">16.33*5</f>
@@ -859,15 +902,15 @@
         <v>13</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F12" s="1" t="n">
         <f aca="false">SUM(C12:E12)</f>
@@ -880,7 +923,7 @@
         <v>2 x X/Y Stepper motor: 17HM19-2004S Nema17 0.9deg 46Ncm 2A</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1" t="n">
         <f aca="false">17.09*2</f>
@@ -904,31 +947,31 @@
         <v>13</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F14" s="1" t="n">
         <f aca="false">SUM(C14:E14)</f>
         <v>0</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F15" s="1" t="n">
         <f aca="false">SUM(C15:E15)</f>
         <v>0</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -937,7 +980,7 @@
         <v>2 x GT2 Pulley 16 Teeth 5mm bore / excellent GT2 pully 16 Teeth (for X/Y steppers)</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>6.88</v>
@@ -963,12 +1006,12 @@
         <v>13</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F17" s="1" t="n">
         <f aca="false">SUM(C17:E17)</f>
@@ -977,10 +1020,10 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>58.4</v>
@@ -995,10 +1038,10 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>51.5</v>
@@ -1013,7 +1056,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>66.4</v>
@@ -1028,7 +1071,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C21" s="1" t="n">
         <f aca="false">3.03*4</f>
@@ -1055,12 +1098,12 @@
         <v>13</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1069,7 +1112,7 @@
         <v>1 x 4m Gates 6mm GT2 Fiber Glass Reinforced Belt</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>18.04</v>
@@ -1092,15 +1135,15 @@
         <v>13</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>9.28</v>
@@ -1123,24 +1166,24 @@
         <v>13</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F26" s="1" t="n">
         <f aca="false">SUM(C26:E26)</f>
         <v>0</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" s="2" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1149,7 +1192,7 @@
         <v>SKR v1.3 + TFT35 + 5xTMC2208 Kit</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>54.13</v>
@@ -1172,7 +1215,7 @@
         <v>13</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1181,7 +1224,7 @@
         <v>1 x Mini differential IR Auto leveling sensor / Mini differential IR height sensor</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>14.71</v>
@@ -1204,7 +1247,7 @@
         <v>13</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1213,7 +1256,7 @@
         <v>1 x Power Supply DC 24V 20A/30A - i use it / Meanwell PSU 24V 450W</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>64.15</v>
@@ -1236,7 +1279,7 @@
         <v>13</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1265,12 +1308,12 @@
         <v>13</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>1.55</v>
@@ -1295,7 +1338,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C35" s="1" t="n">
         <f aca="false">2.79*3</f>
@@ -1321,7 +1364,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F36" s="1" t="n">
         <f aca="false">SUM(C36:E36)</f>
@@ -1330,7 +1373,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C37" s="1" t="n">
         <v>2.09</v>
@@ -1353,12 +1396,12 @@
         <v>13</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>3.19</v>
@@ -1381,12 +1424,12 @@
         <v>13</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F39" s="1" t="n">
         <f aca="false">SUM(C39:E39)</f>
@@ -1395,7 +1438,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F40" s="1" t="n">
         <f aca="false">SUM(C40:E40)</f>
@@ -1419,7 +1462,7 @@
         <v>18.66</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1449,15 +1492,15 @@
         <v>13</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>2.1</v>
@@ -1482,7 +1525,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C44" s="1" t="n">
         <f aca="false">1.7*2</f>
@@ -1512,19 +1555,19 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F45" s="1" t="n">
         <f aca="false">SUM(C45:E45)</f>
         <v>0</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F46" s="1" t="n">
         <f aca="false">SUM(C46:E46)</f>
@@ -1533,7 +1576,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F47" s="1" t="n">
         <f aca="false">SUM(C47:E47)</f>
@@ -1542,19 +1585,19 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F48" s="1" t="n">
         <f aca="false">SUM(C48:E48)</f>
         <v>0</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F49" s="1" t="n">
         <f aca="false">SUM(C49:E49)</f>
@@ -1563,7 +1606,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F50" s="1" t="n">
         <f aca="false">SUM(C50:E50)</f>
@@ -1572,7 +1615,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F51" s="1" t="n">
         <f aca="false">SUM(C51:E51)</f>
@@ -1581,7 +1624,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F52" s="1" t="n">
         <f aca="false">SUM(C52:E52)</f>
@@ -1590,7 +1633,7 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F53" s="1" t="n">
         <f aca="false">SUM(C53:E53)</f>
@@ -1599,7 +1642,7 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F54" s="1" t="n">
         <f aca="false">SUM(C54:E54)</f>
@@ -1608,7 +1651,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F55" s="1" t="n">
         <f aca="false">SUM(C55:E55)</f>
@@ -1617,7 +1660,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F56" s="1" t="n">
         <f aca="false">SUM(C56:E56)</f>
@@ -1626,7 +1669,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F57" s="1" t="n">
         <f aca="false">SUM(C57:E57)</f>
@@ -1635,7 +1678,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C58" s="1" t="n">
         <v>41.05</v>
@@ -1650,10 +1693,10 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C59" s="1" t="n">
         <v>57.67</v>
@@ -1676,12 +1719,12 @@
         <v>13</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F60" s="1" t="n">
         <f aca="false">SUM(C60:E60)</f>
@@ -1690,7 +1733,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F61" s="1" t="n">
         <f aca="false">SUM(C61:E61)</f>
@@ -1699,7 +1742,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F62" s="1" t="n">
         <f aca="false">SUM(C62:E62)</f>
@@ -1708,7 +1751,7 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F63" s="1" t="n">
         <f aca="false">SUM(C63:E63)</f>
@@ -1717,7 +1760,7 @@
     </row>
     <row r="65" s="2" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1736,7 +1779,7 @@
         <v>45.91</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1745,7 +1788,7 @@
         <v>BMG Extruder Clone (Plastic Gear)</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C67" s="1" t="n">
         <v>29.19</v>
@@ -1768,12 +1811,12 @@
         <v>13</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F68" s="1" t="n">
         <f aca="false">SUM(C68:E68)</f>
@@ -1786,12 +1829,12 @@
         <v>13</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F69" s="1" t="n">
         <f aca="false">SUM(C69:E69)</f>
@@ -1800,7 +1843,7 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F70" s="1" t="n">
         <f aca="false">SUM(C70:E70)</f>
@@ -1809,19 +1852,19 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F71" s="1" t="n">
         <f aca="false">SUM(C71:E71)</f>
         <v>0</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="73" s="3" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F73" s="3" t="n">
         <f aca="false">SUM(C73:E73)</f>
@@ -1830,7 +1873,7 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F74" s="1" t="n">
         <f aca="false">SUM(C74:E74)</f>
@@ -1839,7 +1882,7 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F75" s="1" t="n">
         <f aca="false">SUM(C75:E75)</f>
@@ -1848,7 +1891,7 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F76" s="1" t="n">
         <f aca="false">SUM(C76:E76)</f>
@@ -1857,7 +1900,7 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F77" s="1" t="n">
         <f aca="false">SUM(C77:E77)</f>
@@ -1866,7 +1909,7 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F78" s="1" t="n">
         <f aca="false">SUM(C78:E78)</f>
@@ -1875,7 +1918,7 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F79" s="1" t="n">
         <f aca="false">SUM(C79:E79)</f>
@@ -1884,7 +1927,7 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F80" s="1" t="n">
         <f aca="false">SUM(C80:E80)</f>
@@ -1893,7 +1936,7 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F81" s="1" t="n">
         <f aca="false">SUM(C81:E81)</f>
@@ -1902,7 +1945,7 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F82" s="1" t="n">
         <f aca="false">SUM(C82:E82)</f>
@@ -1911,7 +1954,7 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F83" s="1" t="n">
         <f aca="false">SUM(C83:E83)</f>
@@ -1920,7 +1963,7 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F84" s="1" t="n">
         <f aca="false">SUM(C84:E84)</f>
@@ -1929,7 +1972,7 @@
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F85" s="1" t="n">
         <f aca="false">SUM(C85:E85)</f>
@@ -1938,7 +1981,7 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F86" s="1" t="n">
         <f aca="false">SUM(C86:E86)</f>
@@ -1947,7 +1990,7 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F87" s="1" t="n">
         <f aca="false">SUM(C87:E87)</f>
@@ -1956,7 +1999,7 @@
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F88" s="1" t="n">
         <f aca="false">SUM(C88:E88)</f>
@@ -1965,7 +2008,7 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F89" s="1" t="n">
         <f aca="false">SUM(C89:E89)</f>
@@ -1974,7 +2017,7 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F90" s="1" t="n">
         <f aca="false">SUM(C90:E90)</f>
@@ -1983,7 +2026,7 @@
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F91" s="1" t="n">
         <f aca="false">SUM(C91:E91)</f>
@@ -1992,7 +2035,7 @@
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F92" s="1" t="n">
         <f aca="false">SUM(C92:E92)</f>
@@ -2001,7 +2044,7 @@
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F93" s="1" t="n">
         <f aca="false">SUM(C93:E93)</f>
@@ -2010,7 +2053,7 @@
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F94" s="1" t="n">
         <f aca="false">SUM(C94:E94)</f>
@@ -2019,7 +2062,7 @@
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F95" s="1" t="n">
         <f aca="false">SUM(C95:E95)</f>
@@ -2028,7 +2071,7 @@
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F96" s="1" t="n">
         <f aca="false">SUM(C96:E96)</f>
@@ -2037,7 +2080,7 @@
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F97" s="1" t="n">
         <f aca="false">SUM(C97:E97)</f>
@@ -2046,7 +2089,7 @@
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F98" s="1" t="n">
         <f aca="false">SUM(C98:E98)</f>
@@ -2055,7 +2098,7 @@
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F99" s="1" t="n">
         <f aca="false">SUM(C99:E99)</f>
@@ -2064,7 +2107,7 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F100" s="1" t="n">
         <f aca="false">SUM(C100:E100)</f>
@@ -2073,7 +2116,7 @@
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F101" s="1" t="n">
         <f aca="false">SUM(C101:E101)</f>
@@ -2082,7 +2125,7 @@
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F102" s="1" t="n">
         <f aca="false">SUM(C102:E102)</f>
@@ -2091,7 +2134,7 @@
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F103" s="1" t="n">
         <f aca="false">SUM(C103:E103)</f>
@@ -2100,7 +2143,7 @@
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F104" s="1" t="n">
         <f aca="false">SUM(C104:E104)</f>
@@ -2109,7 +2152,7 @@
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F105" s="1" t="n">
         <f aca="false">SUM(C105:E105)</f>
@@ -2118,7 +2161,7 @@
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F106" s="1" t="n">
         <f aca="false">SUM(C106:E106)</f>
@@ -2127,7 +2170,7 @@
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F107" s="1" t="n">
         <f aca="false">SUM(C107:E107)</f>
@@ -2136,7 +2179,7 @@
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F108" s="1" t="n">
         <f aca="false">SUM(C108:E108)</f>
@@ -2145,7 +2188,7 @@
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F109" s="1" t="n">
         <f aca="false">SUM(C109:E109)</f>
@@ -2154,7 +2197,7 @@
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F110" s="1" t="n">
         <f aca="false">SUM(C110:E110)</f>
@@ -2163,7 +2206,7 @@
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F111" s="1" t="n">
         <f aca="false">SUM(C111:E111)</f>
@@ -2172,7 +2215,7 @@
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F112" s="1" t="n">
         <f aca="false">SUM(C112:E112)</f>
@@ -2181,7 +2224,7 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C113" s="1" t="n">
         <v>3.34</v>
@@ -2201,12 +2244,12 @@
         <v>13</v>
       </c>
       <c r="J113" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C114" s="1" t="n">
         <v>1.64</v>
@@ -2231,10 +2274,10 @@
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C115" s="1" t="n">
         <v>0.88</v>
@@ -2257,36 +2300,36 @@
         <v>13</v>
       </c>
       <c r="J115" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F116" s="1" t="n">
         <f aca="false">SUM(C116:E116)</f>
         <v>0</v>
       </c>
       <c r="J116" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F117" s="1" t="n">
         <f aca="false">SUM(C117:E117)</f>
         <v>0</v>
       </c>
       <c r="J117" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F118" s="1" t="n">
         <f aca="false">SUM(C118:E118)</f>
@@ -2295,7 +2338,7 @@
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F119" s="1" t="n">
         <f aca="false">SUM(C119:E119)</f>
@@ -2304,7 +2347,7 @@
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F120" s="1" t="n">
         <f aca="false">SUM(C120:E120)</f>
@@ -2313,7 +2356,7 @@
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C121" s="1" t="n">
         <v>2.91</v>
@@ -2341,7 +2384,7 @@
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F122" s="1" t="n">
         <f aca="false">SUM(C122:E122)</f>
@@ -2350,7 +2393,7 @@
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F123" s="1" t="n">
         <f aca="false">SUM(C123:E123)</f>
@@ -2359,7 +2402,7 @@
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F124" s="1" t="n">
         <f aca="false">SUM(C124:E124)</f>
@@ -2368,7 +2411,7 @@
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F125" s="1" t="n">
         <f aca="false">SUM(C125:E125)</f>
@@ -2377,7 +2420,7 @@
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F126" s="1" t="n">
         <f aca="false">SUM(C126:E126)</f>
@@ -2386,7 +2429,7 @@
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F127" s="1" t="n">
         <f aca="false">SUM(C127:E127)</f>
@@ -2395,7 +2438,7 @@
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F128" s="1" t="n">
         <f aca="false">SUM(C128:E128)</f>
@@ -2404,7 +2447,7 @@
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F129" s="1" t="n">
         <f aca="false">SUM(C129:E129)</f>
@@ -2413,7 +2456,7 @@
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F130" s="1" t="n">
         <f aca="false">SUM(C130:E130)</f>
@@ -2422,7 +2465,7 @@
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F131" s="1" t="n">
         <f aca="false">SUM(C131:E131)</f>
@@ -2431,7 +2474,7 @@
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F132" s="1" t="n">
         <f aca="false">SUM(C132:E132)</f>
@@ -2440,7 +2483,7 @@
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F133" s="1" t="n">
         <f aca="false">SUM(C133:E133)</f>
@@ -2449,7 +2492,7 @@
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F134" s="1" t="n">
         <f aca="false">SUM(C134:E134)</f>
@@ -2458,7 +2501,7 @@
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F135" s="1" t="n">
         <f aca="false">SUM(C135:E135)</f>
@@ -2467,12 +2510,12 @@
     </row>
     <row r="137" s="2" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C138" s="1" t="n">
         <v>12.69</v>
@@ -2497,7 +2540,7 @@
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F139" s="1" t="n">
         <f aca="false">SUM(C139:E139)</f>
@@ -2506,7 +2549,7 @@
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F140" s="1" t="n">
         <f aca="false">SUM(C140:E140)</f>
@@ -2515,7 +2558,7 @@
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F141" s="1" t="n">
         <f aca="false">SUM(C141:E141)</f>
@@ -2524,7 +2567,7 @@
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C142" s="1" t="n">
         <v>3.02</v>
@@ -2547,12 +2590,12 @@
         <v>13</v>
       </c>
       <c r="J142" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F143" s="1" t="n">
         <f aca="false">SUM(C143:E143)</f>
@@ -2561,7 +2604,7 @@
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F144" s="1" t="n">
         <f aca="false">SUM(C144:E144)</f>
@@ -2570,7 +2613,7 @@
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F145" s="1" t="n">
         <f aca="false">SUM(C145:E145)</f>
@@ -2579,7 +2622,7 @@
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F146" s="1" t="n">
         <f aca="false">SUM(C146:E146)</f>
@@ -2588,7 +2631,7 @@
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F147" s="1" t="n">
         <f aca="false">SUM(C147:E147)</f>
@@ -2597,7 +2640,7 @@
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F148" s="1" t="n">
         <f aca="false">SUM(C148:E148)</f>
@@ -2606,7 +2649,7 @@
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F149" s="1" t="n">
         <f aca="false">SUM(C149:E149)</f>
@@ -2615,7 +2658,7 @@
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F150" s="1" t="n">
         <f aca="false">SUM(C150:E150)</f>
@@ -2624,7 +2667,7 @@
     </row>
     <row r="152" s="3" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="153" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2662,1056 +2705,41 @@
         <v>11</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="B154" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C154" s="0" t="n">
+    <row r="154" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B154" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C154" s="5" t="n">
         <v>3.04</v>
       </c>
-      <c r="D154" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E154" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F154" s="0" t="n">
+      <c r="D154" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E154" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F154" s="5" t="n">
         <v>3.04</v>
       </c>
-      <c r="G154" s="0" t="n">
+      <c r="G154" s="5" t="n">
         <v>3.04</v>
       </c>
-      <c r="H154" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="I154" s="0"/>
-      <c r="J154" s="0"/>
-      <c r="K154" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="L154" s="0"/>
-      <c r="M154" s="0"/>
-      <c r="N154" s="0"/>
-      <c r="O154" s="0"/>
-      <c r="P154" s="0"/>
-      <c r="Q154" s="0"/>
-      <c r="R154" s="0"/>
-      <c r="S154" s="0"/>
-      <c r="T154" s="0"/>
-      <c r="U154" s="0"/>
-      <c r="V154" s="0"/>
-      <c r="W154" s="0"/>
-      <c r="X154" s="0"/>
-      <c r="Y154" s="0"/>
-      <c r="Z154" s="0"/>
-      <c r="AA154" s="0"/>
-      <c r="AB154" s="0"/>
-      <c r="AC154" s="0"/>
-      <c r="AD154" s="0"/>
-      <c r="AE154" s="0"/>
-      <c r="AF154" s="0"/>
-      <c r="AG154" s="0"/>
-      <c r="AH154" s="0"/>
-      <c r="AI154" s="0"/>
-      <c r="AJ154" s="0"/>
-      <c r="AK154" s="0"/>
-      <c r="AL154" s="0"/>
-      <c r="AM154" s="0"/>
-      <c r="AN154" s="0"/>
-      <c r="AO154" s="0"/>
-      <c r="AP154" s="0"/>
-      <c r="AQ154" s="0"/>
-      <c r="AR154" s="0"/>
-      <c r="AS154" s="0"/>
-      <c r="AT154" s="0"/>
-      <c r="AU154" s="0"/>
-      <c r="AV154" s="0"/>
-      <c r="AW154" s="0"/>
-      <c r="AX154" s="0"/>
-      <c r="AY154" s="0"/>
-      <c r="AZ154" s="0"/>
-      <c r="BA154" s="0"/>
-      <c r="BB154" s="0"/>
-      <c r="BC154" s="0"/>
-      <c r="BD154" s="0"/>
-      <c r="BE154" s="0"/>
-      <c r="BF154" s="0"/>
-      <c r="BG154" s="0"/>
-      <c r="BH154" s="0"/>
-      <c r="BI154" s="0"/>
-      <c r="BJ154" s="0"/>
-      <c r="BK154" s="0"/>
-      <c r="BL154" s="0"/>
-      <c r="BM154" s="0"/>
-      <c r="BN154" s="0"/>
-      <c r="BO154" s="0"/>
-      <c r="BP154" s="0"/>
-      <c r="BQ154" s="0"/>
-      <c r="BR154" s="0"/>
-      <c r="BS154" s="0"/>
-      <c r="BT154" s="0"/>
-      <c r="BU154" s="0"/>
-      <c r="BV154" s="0"/>
-      <c r="BW154" s="0"/>
-      <c r="BX154" s="0"/>
-      <c r="BY154" s="0"/>
-      <c r="BZ154" s="0"/>
-      <c r="CA154" s="0"/>
-      <c r="CB154" s="0"/>
-      <c r="CC154" s="0"/>
-      <c r="CD154" s="0"/>
-      <c r="CE154" s="0"/>
-      <c r="CF154" s="0"/>
-      <c r="CG154" s="0"/>
-      <c r="CH154" s="0"/>
-      <c r="CI154" s="0"/>
-      <c r="CJ154" s="0"/>
-      <c r="CK154" s="0"/>
-      <c r="CL154" s="0"/>
-      <c r="CM154" s="0"/>
-      <c r="CN154" s="0"/>
-      <c r="CO154" s="0"/>
-      <c r="CP154" s="0"/>
-      <c r="CQ154" s="0"/>
-      <c r="CR154" s="0"/>
-      <c r="CS154" s="0"/>
-      <c r="CT154" s="0"/>
-      <c r="CU154" s="0"/>
-      <c r="CV154" s="0"/>
-      <c r="CW154" s="0"/>
-      <c r="CX154" s="0"/>
-      <c r="CY154" s="0"/>
-      <c r="CZ154" s="0"/>
-      <c r="DA154" s="0"/>
-      <c r="DB154" s="0"/>
-      <c r="DC154" s="0"/>
-      <c r="DD154" s="0"/>
-      <c r="DE154" s="0"/>
-      <c r="DF154" s="0"/>
-      <c r="DG154" s="0"/>
-      <c r="DH154" s="0"/>
-      <c r="DI154" s="0"/>
-      <c r="DJ154" s="0"/>
-      <c r="DK154" s="0"/>
-      <c r="DL154" s="0"/>
-      <c r="DM154" s="0"/>
-      <c r="DN154" s="0"/>
-      <c r="DO154" s="0"/>
-      <c r="DP154" s="0"/>
-      <c r="DQ154" s="0"/>
-      <c r="DR154" s="0"/>
-      <c r="DS154" s="0"/>
-      <c r="DT154" s="0"/>
-      <c r="DU154" s="0"/>
-      <c r="DV154" s="0"/>
-      <c r="DW154" s="0"/>
-      <c r="DX154" s="0"/>
-      <c r="DY154" s="0"/>
-      <c r="DZ154" s="0"/>
-      <c r="EA154" s="0"/>
-      <c r="EB154" s="0"/>
-      <c r="EC154" s="0"/>
-      <c r="ED154" s="0"/>
-      <c r="EE154" s="0"/>
-      <c r="EF154" s="0"/>
-      <c r="EG154" s="0"/>
-      <c r="EH154" s="0"/>
-      <c r="EI154" s="0"/>
-      <c r="EJ154" s="0"/>
-      <c r="EK154" s="0"/>
-      <c r="EL154" s="0"/>
-      <c r="EM154" s="0"/>
-      <c r="EN154" s="0"/>
-      <c r="EO154" s="0"/>
-      <c r="EP154" s="0"/>
-      <c r="EQ154" s="0"/>
-      <c r="ER154" s="0"/>
-      <c r="ES154" s="0"/>
-      <c r="ET154" s="0"/>
-      <c r="EU154" s="0"/>
-      <c r="EV154" s="0"/>
-      <c r="EW154" s="0"/>
-      <c r="EX154" s="0"/>
-      <c r="EY154" s="0"/>
-      <c r="EZ154" s="0"/>
-      <c r="FA154" s="0"/>
-      <c r="FB154" s="0"/>
-      <c r="FC154" s="0"/>
-      <c r="FD154" s="0"/>
-      <c r="FE154" s="0"/>
-      <c r="FF154" s="0"/>
-      <c r="FG154" s="0"/>
-      <c r="FH154" s="0"/>
-      <c r="FI154" s="0"/>
-      <c r="FJ154" s="0"/>
-      <c r="FK154" s="0"/>
-      <c r="FL154" s="0"/>
-      <c r="FM154" s="0"/>
-      <c r="FN154" s="0"/>
-      <c r="FO154" s="0"/>
-      <c r="FP154" s="0"/>
-      <c r="FQ154" s="0"/>
-      <c r="FR154" s="0"/>
-      <c r="FS154" s="0"/>
-      <c r="FT154" s="0"/>
-      <c r="FU154" s="0"/>
-      <c r="FV154" s="0"/>
-      <c r="FW154" s="0"/>
-      <c r="FX154" s="0"/>
-      <c r="FY154" s="0"/>
-      <c r="FZ154" s="0"/>
-      <c r="GA154" s="0"/>
-      <c r="GB154" s="0"/>
-      <c r="GC154" s="0"/>
-      <c r="GD154" s="0"/>
-      <c r="GE154" s="0"/>
-      <c r="GF154" s="0"/>
-      <c r="GG154" s="0"/>
-      <c r="GH154" s="0"/>
-      <c r="GI154" s="0"/>
-      <c r="GJ154" s="0"/>
-      <c r="GK154" s="0"/>
-      <c r="GL154" s="0"/>
-      <c r="GM154" s="0"/>
-      <c r="GN154" s="0"/>
-      <c r="GO154" s="0"/>
-      <c r="GP154" s="0"/>
-      <c r="GQ154" s="0"/>
-      <c r="GR154" s="0"/>
-      <c r="GS154" s="0"/>
-      <c r="GT154" s="0"/>
-      <c r="GU154" s="0"/>
-      <c r="GV154" s="0"/>
-      <c r="GW154" s="0"/>
-      <c r="GX154" s="0"/>
-      <c r="GY154" s="0"/>
-      <c r="GZ154" s="0"/>
-      <c r="HA154" s="0"/>
-      <c r="HB154" s="0"/>
-      <c r="HC154" s="0"/>
-      <c r="HD154" s="0"/>
-      <c r="HE154" s="0"/>
-      <c r="HF154" s="0"/>
-      <c r="HG154" s="0"/>
-      <c r="HH154" s="0"/>
-      <c r="HI154" s="0"/>
-      <c r="HJ154" s="0"/>
-      <c r="HK154" s="0"/>
-      <c r="HL154" s="0"/>
-      <c r="HM154" s="0"/>
-      <c r="HN154" s="0"/>
-      <c r="HO154" s="0"/>
-      <c r="HP154" s="0"/>
-      <c r="HQ154" s="0"/>
-      <c r="HR154" s="0"/>
-      <c r="HS154" s="0"/>
-      <c r="HT154" s="0"/>
-      <c r="HU154" s="0"/>
-      <c r="HV154" s="0"/>
-      <c r="HW154" s="0"/>
-      <c r="HX154" s="0"/>
-      <c r="HY154" s="0"/>
-      <c r="HZ154" s="0"/>
-      <c r="IA154" s="0"/>
-      <c r="IB154" s="0"/>
-      <c r="IC154" s="0"/>
-      <c r="ID154" s="0"/>
-      <c r="IE154" s="0"/>
-      <c r="IF154" s="0"/>
-      <c r="IG154" s="0"/>
-      <c r="IH154" s="0"/>
-      <c r="II154" s="0"/>
-      <c r="IJ154" s="0"/>
-      <c r="IK154" s="0"/>
-      <c r="IL154" s="0"/>
-      <c r="IM154" s="0"/>
-      <c r="IN154" s="0"/>
-      <c r="IO154" s="0"/>
-      <c r="IP154" s="0"/>
-      <c r="IQ154" s="0"/>
-      <c r="IR154" s="0"/>
-      <c r="IS154" s="0"/>
-      <c r="IT154" s="0"/>
-      <c r="IU154" s="0"/>
-      <c r="IV154" s="0"/>
-      <c r="IW154" s="0"/>
-      <c r="IX154" s="0"/>
-      <c r="IY154" s="0"/>
-      <c r="IZ154" s="0"/>
-      <c r="JA154" s="0"/>
-      <c r="JB154" s="0"/>
-      <c r="JC154" s="0"/>
-      <c r="JD154" s="0"/>
-      <c r="JE154" s="0"/>
-      <c r="JF154" s="0"/>
-      <c r="JG154" s="0"/>
-      <c r="JH154" s="0"/>
-      <c r="JI154" s="0"/>
-      <c r="JJ154" s="0"/>
-      <c r="JK154" s="0"/>
-      <c r="JL154" s="0"/>
-      <c r="JM154" s="0"/>
-      <c r="JN154" s="0"/>
-      <c r="JO154" s="0"/>
-      <c r="JP154" s="0"/>
-      <c r="JQ154" s="0"/>
-      <c r="JR154" s="0"/>
-      <c r="JS154" s="0"/>
-      <c r="JT154" s="0"/>
-      <c r="JU154" s="0"/>
-      <c r="JV154" s="0"/>
-      <c r="JW154" s="0"/>
-      <c r="JX154" s="0"/>
-      <c r="JY154" s="0"/>
-      <c r="JZ154" s="0"/>
-      <c r="KA154" s="0"/>
-      <c r="KB154" s="0"/>
-      <c r="KC154" s="0"/>
-      <c r="KD154" s="0"/>
-      <c r="KE154" s="0"/>
-      <c r="KF154" s="0"/>
-      <c r="KG154" s="0"/>
-      <c r="KH154" s="0"/>
-      <c r="KI154" s="0"/>
-      <c r="KJ154" s="0"/>
-      <c r="KK154" s="0"/>
-      <c r="KL154" s="0"/>
-      <c r="KM154" s="0"/>
-      <c r="KN154" s="0"/>
-      <c r="KO154" s="0"/>
-      <c r="KP154" s="0"/>
-      <c r="KQ154" s="0"/>
-      <c r="KR154" s="0"/>
-      <c r="KS154" s="0"/>
-      <c r="KT154" s="0"/>
-      <c r="KU154" s="0"/>
-      <c r="KV154" s="0"/>
-      <c r="KW154" s="0"/>
-      <c r="KX154" s="0"/>
-      <c r="KY154" s="0"/>
-      <c r="KZ154" s="0"/>
-      <c r="LA154" s="0"/>
-      <c r="LB154" s="0"/>
-      <c r="LC154" s="0"/>
-      <c r="LD154" s="0"/>
-      <c r="LE154" s="0"/>
-      <c r="LF154" s="0"/>
-      <c r="LG154" s="0"/>
-      <c r="LH154" s="0"/>
-      <c r="LI154" s="0"/>
-      <c r="LJ154" s="0"/>
-      <c r="LK154" s="0"/>
-      <c r="LL154" s="0"/>
-      <c r="LM154" s="0"/>
-      <c r="LN154" s="0"/>
-      <c r="LO154" s="0"/>
-      <c r="LP154" s="0"/>
-      <c r="LQ154" s="0"/>
-      <c r="LR154" s="0"/>
-      <c r="LS154" s="0"/>
-      <c r="LT154" s="0"/>
-      <c r="LU154" s="0"/>
-      <c r="LV154" s="0"/>
-      <c r="LW154" s="0"/>
-      <c r="LX154" s="0"/>
-      <c r="LY154" s="0"/>
-      <c r="LZ154" s="0"/>
-      <c r="MA154" s="0"/>
-      <c r="MB154" s="0"/>
-      <c r="MC154" s="0"/>
-      <c r="MD154" s="0"/>
-      <c r="ME154" s="0"/>
-      <c r="MF154" s="0"/>
-      <c r="MG154" s="0"/>
-      <c r="MH154" s="0"/>
-      <c r="MI154" s="0"/>
-      <c r="MJ154" s="0"/>
-      <c r="MK154" s="0"/>
-      <c r="ML154" s="0"/>
-      <c r="MM154" s="0"/>
-      <c r="MN154" s="0"/>
-      <c r="MO154" s="0"/>
-      <c r="MP154" s="0"/>
-      <c r="MQ154" s="0"/>
-      <c r="MR154" s="0"/>
-      <c r="MS154" s="0"/>
-      <c r="MT154" s="0"/>
-      <c r="MU154" s="0"/>
-      <c r="MV154" s="0"/>
-      <c r="MW154" s="0"/>
-      <c r="MX154" s="0"/>
-      <c r="MY154" s="0"/>
-      <c r="MZ154" s="0"/>
-      <c r="NA154" s="0"/>
-      <c r="NB154" s="0"/>
-      <c r="NC154" s="0"/>
-      <c r="ND154" s="0"/>
-      <c r="NE154" s="0"/>
-      <c r="NF154" s="0"/>
-      <c r="NG154" s="0"/>
-      <c r="NH154" s="0"/>
-      <c r="NI154" s="0"/>
-      <c r="NJ154" s="0"/>
-      <c r="NK154" s="0"/>
-      <c r="NL154" s="0"/>
-      <c r="NM154" s="0"/>
-      <c r="NN154" s="0"/>
-      <c r="NO154" s="0"/>
-      <c r="NP154" s="0"/>
-      <c r="NQ154" s="0"/>
-      <c r="NR154" s="0"/>
-      <c r="NS154" s="0"/>
-      <c r="NT154" s="0"/>
-      <c r="NU154" s="0"/>
-      <c r="NV154" s="0"/>
-      <c r="NW154" s="0"/>
-      <c r="NX154" s="0"/>
-      <c r="NY154" s="0"/>
-      <c r="NZ154" s="0"/>
-      <c r="OA154" s="0"/>
-      <c r="OB154" s="0"/>
-      <c r="OC154" s="0"/>
-      <c r="OD154" s="0"/>
-      <c r="OE154" s="0"/>
-      <c r="OF154" s="0"/>
-      <c r="OG154" s="0"/>
-      <c r="OH154" s="0"/>
-      <c r="OI154" s="0"/>
-      <c r="OJ154" s="0"/>
-      <c r="OK154" s="0"/>
-      <c r="OL154" s="0"/>
-      <c r="OM154" s="0"/>
-      <c r="ON154" s="0"/>
-      <c r="OO154" s="0"/>
-      <c r="OP154" s="0"/>
-      <c r="OQ154" s="0"/>
-      <c r="OR154" s="0"/>
-      <c r="OS154" s="0"/>
-      <c r="OT154" s="0"/>
-      <c r="OU154" s="0"/>
-      <c r="OV154" s="0"/>
-      <c r="OW154" s="0"/>
-      <c r="OX154" s="0"/>
-      <c r="OY154" s="0"/>
-      <c r="OZ154" s="0"/>
-      <c r="PA154" s="0"/>
-      <c r="PB154" s="0"/>
-      <c r="PC154" s="0"/>
-      <c r="PD154" s="0"/>
-      <c r="PE154" s="0"/>
-      <c r="PF154" s="0"/>
-      <c r="PG154" s="0"/>
-      <c r="PH154" s="0"/>
-      <c r="PI154" s="0"/>
-      <c r="PJ154" s="0"/>
-      <c r="PK154" s="0"/>
-      <c r="PL154" s="0"/>
-      <c r="PM154" s="0"/>
-      <c r="PN154" s="0"/>
-      <c r="PO154" s="0"/>
-      <c r="PP154" s="0"/>
-      <c r="PQ154" s="0"/>
-      <c r="PR154" s="0"/>
-      <c r="PS154" s="0"/>
-      <c r="PT154" s="0"/>
-      <c r="PU154" s="0"/>
-      <c r="PV154" s="0"/>
-      <c r="PW154" s="0"/>
-      <c r="PX154" s="0"/>
-      <c r="PY154" s="0"/>
-      <c r="PZ154" s="0"/>
-      <c r="QA154" s="0"/>
-      <c r="QB154" s="0"/>
-      <c r="QC154" s="0"/>
-      <c r="QD154" s="0"/>
-      <c r="QE154" s="0"/>
-      <c r="QF154" s="0"/>
-      <c r="QG154" s="0"/>
-      <c r="QH154" s="0"/>
-      <c r="QI154" s="0"/>
-      <c r="QJ154" s="0"/>
-      <c r="QK154" s="0"/>
-      <c r="QL154" s="0"/>
-      <c r="QM154" s="0"/>
-      <c r="QN154" s="0"/>
-      <c r="QO154" s="0"/>
-      <c r="QP154" s="0"/>
-      <c r="QQ154" s="0"/>
-      <c r="QR154" s="0"/>
-      <c r="QS154" s="0"/>
-      <c r="QT154" s="0"/>
-      <c r="QU154" s="0"/>
-      <c r="QV154" s="0"/>
-      <c r="QW154" s="0"/>
-      <c r="QX154" s="0"/>
-      <c r="QY154" s="0"/>
-      <c r="QZ154" s="0"/>
-      <c r="RA154" s="0"/>
-      <c r="RB154" s="0"/>
-      <c r="RC154" s="0"/>
-      <c r="RD154" s="0"/>
-      <c r="RE154" s="0"/>
-      <c r="RF154" s="0"/>
-      <c r="RG154" s="0"/>
-      <c r="RH154" s="0"/>
-      <c r="RI154" s="0"/>
-      <c r="RJ154" s="0"/>
-      <c r="RK154" s="0"/>
-      <c r="RL154" s="0"/>
-      <c r="RM154" s="0"/>
-      <c r="RN154" s="0"/>
-      <c r="RO154" s="0"/>
-      <c r="RP154" s="0"/>
-      <c r="RQ154" s="0"/>
-      <c r="RR154" s="0"/>
-      <c r="RS154" s="0"/>
-      <c r="RT154" s="0"/>
-      <c r="RU154" s="0"/>
-      <c r="RV154" s="0"/>
-      <c r="RW154" s="0"/>
-      <c r="RX154" s="0"/>
-      <c r="RY154" s="0"/>
-      <c r="RZ154" s="0"/>
-      <c r="SA154" s="0"/>
-      <c r="SB154" s="0"/>
-      <c r="SC154" s="0"/>
-      <c r="SD154" s="0"/>
-      <c r="SE154" s="0"/>
-      <c r="SF154" s="0"/>
-      <c r="SG154" s="0"/>
-      <c r="SH154" s="0"/>
-      <c r="SI154" s="0"/>
-      <c r="SJ154" s="0"/>
-      <c r="SK154" s="0"/>
-      <c r="SL154" s="0"/>
-      <c r="SM154" s="0"/>
-      <c r="SN154" s="0"/>
-      <c r="SO154" s="0"/>
-      <c r="SP154" s="0"/>
-      <c r="SQ154" s="0"/>
-      <c r="SR154" s="0"/>
-      <c r="SS154" s="0"/>
-      <c r="ST154" s="0"/>
-      <c r="SU154" s="0"/>
-      <c r="SV154" s="0"/>
-      <c r="SW154" s="0"/>
-      <c r="SX154" s="0"/>
-      <c r="SY154" s="0"/>
-      <c r="SZ154" s="0"/>
-      <c r="TA154" s="0"/>
-      <c r="TB154" s="0"/>
-      <c r="TC154" s="0"/>
-      <c r="TD154" s="0"/>
-      <c r="TE154" s="0"/>
-      <c r="TF154" s="0"/>
-      <c r="TG154" s="0"/>
-      <c r="TH154" s="0"/>
-      <c r="TI154" s="0"/>
-      <c r="TJ154" s="0"/>
-      <c r="TK154" s="0"/>
-      <c r="TL154" s="0"/>
-      <c r="TM154" s="0"/>
-      <c r="TN154" s="0"/>
-      <c r="TO154" s="0"/>
-      <c r="TP154" s="0"/>
-      <c r="TQ154" s="0"/>
-      <c r="TR154" s="0"/>
-      <c r="TS154" s="0"/>
-      <c r="TT154" s="0"/>
-      <c r="TU154" s="0"/>
-      <c r="TV154" s="0"/>
-      <c r="TW154" s="0"/>
-      <c r="TX154" s="0"/>
-      <c r="TY154" s="0"/>
-      <c r="TZ154" s="0"/>
-      <c r="UA154" s="0"/>
-      <c r="UB154" s="0"/>
-      <c r="UC154" s="0"/>
-      <c r="UD154" s="0"/>
-      <c r="UE154" s="0"/>
-      <c r="UF154" s="0"/>
-      <c r="UG154" s="0"/>
-      <c r="UH154" s="0"/>
-      <c r="UI154" s="0"/>
-      <c r="UJ154" s="0"/>
-      <c r="UK154" s="0"/>
-      <c r="UL154" s="0"/>
-      <c r="UM154" s="0"/>
-      <c r="UN154" s="0"/>
-      <c r="UO154" s="0"/>
-      <c r="UP154" s="0"/>
-      <c r="UQ154" s="0"/>
-      <c r="UR154" s="0"/>
-      <c r="US154" s="0"/>
-      <c r="UT154" s="0"/>
-      <c r="UU154" s="0"/>
-      <c r="UV154" s="0"/>
-      <c r="UW154" s="0"/>
-      <c r="UX154" s="0"/>
-      <c r="UY154" s="0"/>
-      <c r="UZ154" s="0"/>
-      <c r="VA154" s="0"/>
-      <c r="VB154" s="0"/>
-      <c r="VC154" s="0"/>
-      <c r="VD154" s="0"/>
-      <c r="VE154" s="0"/>
-      <c r="VF154" s="0"/>
-      <c r="VG154" s="0"/>
-      <c r="VH154" s="0"/>
-      <c r="VI154" s="0"/>
-      <c r="VJ154" s="0"/>
-      <c r="VK154" s="0"/>
-      <c r="VL154" s="0"/>
-      <c r="VM154" s="0"/>
-      <c r="VN154" s="0"/>
-      <c r="VO154" s="0"/>
-      <c r="VP154" s="0"/>
-      <c r="VQ154" s="0"/>
-      <c r="VR154" s="0"/>
-      <c r="VS154" s="0"/>
-      <c r="VT154" s="0"/>
-      <c r="VU154" s="0"/>
-      <c r="VV154" s="0"/>
-      <c r="VW154" s="0"/>
-      <c r="VX154" s="0"/>
-      <c r="VY154" s="0"/>
-      <c r="VZ154" s="0"/>
-      <c r="WA154" s="0"/>
-      <c r="WB154" s="0"/>
-      <c r="WC154" s="0"/>
-      <c r="WD154" s="0"/>
-      <c r="WE154" s="0"/>
-      <c r="WF154" s="0"/>
-      <c r="WG154" s="0"/>
-      <c r="WH154" s="0"/>
-      <c r="WI154" s="0"/>
-      <c r="WJ154" s="0"/>
-      <c r="WK154" s="0"/>
-      <c r="WL154" s="0"/>
-      <c r="WM154" s="0"/>
-      <c r="WN154" s="0"/>
-      <c r="WO154" s="0"/>
-      <c r="WP154" s="0"/>
-      <c r="WQ154" s="0"/>
-      <c r="WR154" s="0"/>
-      <c r="WS154" s="0"/>
-      <c r="WT154" s="0"/>
-      <c r="WU154" s="0"/>
-      <c r="WV154" s="0"/>
-      <c r="WW154" s="0"/>
-      <c r="WX154" s="0"/>
-      <c r="WY154" s="0"/>
-      <c r="WZ154" s="0"/>
-      <c r="XA154" s="0"/>
-      <c r="XB154" s="0"/>
-      <c r="XC154" s="0"/>
-      <c r="XD154" s="0"/>
-      <c r="XE154" s="0"/>
-      <c r="XF154" s="0"/>
-      <c r="XG154" s="0"/>
-      <c r="XH154" s="0"/>
-      <c r="XI154" s="0"/>
-      <c r="XJ154" s="0"/>
-      <c r="XK154" s="0"/>
-      <c r="XL154" s="0"/>
-      <c r="XM154" s="0"/>
-      <c r="XN154" s="0"/>
-      <c r="XO154" s="0"/>
-      <c r="XP154" s="0"/>
-      <c r="XQ154" s="0"/>
-      <c r="XR154" s="0"/>
-      <c r="XS154" s="0"/>
-      <c r="XT154" s="0"/>
-      <c r="XU154" s="0"/>
-      <c r="XV154" s="0"/>
-      <c r="XW154" s="0"/>
-      <c r="XX154" s="0"/>
-      <c r="XY154" s="0"/>
-      <c r="XZ154" s="0"/>
-      <c r="YA154" s="0"/>
-      <c r="YB154" s="0"/>
-      <c r="YC154" s="0"/>
-      <c r="YD154" s="0"/>
-      <c r="YE154" s="0"/>
-      <c r="YF154" s="0"/>
-      <c r="YG154" s="0"/>
-      <c r="YH154" s="0"/>
-      <c r="YI154" s="0"/>
-      <c r="YJ154" s="0"/>
-      <c r="YK154" s="0"/>
-      <c r="YL154" s="0"/>
-      <c r="YM154" s="0"/>
-      <c r="YN154" s="0"/>
-      <c r="YO154" s="0"/>
-      <c r="YP154" s="0"/>
-      <c r="YQ154" s="0"/>
-      <c r="YR154" s="0"/>
-      <c r="YS154" s="0"/>
-      <c r="YT154" s="0"/>
-      <c r="YU154" s="0"/>
-      <c r="YV154" s="0"/>
-      <c r="YW154" s="0"/>
-      <c r="YX154" s="0"/>
-      <c r="YY154" s="0"/>
-      <c r="YZ154" s="0"/>
-      <c r="ZA154" s="0"/>
-      <c r="ZB154" s="0"/>
-      <c r="ZC154" s="0"/>
-      <c r="ZD154" s="0"/>
-      <c r="ZE154" s="0"/>
-      <c r="ZF154" s="0"/>
-      <c r="ZG154" s="0"/>
-      <c r="ZH154" s="0"/>
-      <c r="ZI154" s="0"/>
-      <c r="ZJ154" s="0"/>
-      <c r="ZK154" s="0"/>
-      <c r="ZL154" s="0"/>
-      <c r="ZM154" s="0"/>
-      <c r="ZN154" s="0"/>
-      <c r="ZO154" s="0"/>
-      <c r="ZP154" s="0"/>
-      <c r="ZQ154" s="0"/>
-      <c r="ZR154" s="0"/>
-      <c r="ZS154" s="0"/>
-      <c r="ZT154" s="0"/>
-      <c r="ZU154" s="0"/>
-      <c r="ZV154" s="0"/>
-      <c r="ZW154" s="0"/>
-      <c r="ZX154" s="0"/>
-      <c r="ZY154" s="0"/>
-      <c r="ZZ154" s="0"/>
-      <c r="AAA154" s="0"/>
-      <c r="AAB154" s="0"/>
-      <c r="AAC154" s="0"/>
-      <c r="AAD154" s="0"/>
-      <c r="AAE154" s="0"/>
-      <c r="AAF154" s="0"/>
-      <c r="AAG154" s="0"/>
-      <c r="AAH154" s="0"/>
-      <c r="AAI154" s="0"/>
-      <c r="AAJ154" s="0"/>
-      <c r="AAK154" s="0"/>
-      <c r="AAL154" s="0"/>
-      <c r="AAM154" s="0"/>
-      <c r="AAN154" s="0"/>
-      <c r="AAO154" s="0"/>
-      <c r="AAP154" s="0"/>
-      <c r="AAQ154" s="0"/>
-      <c r="AAR154" s="0"/>
-      <c r="AAS154" s="0"/>
-      <c r="AAT154" s="0"/>
-      <c r="AAU154" s="0"/>
-      <c r="AAV154" s="0"/>
-      <c r="AAW154" s="0"/>
-      <c r="AAX154" s="0"/>
-      <c r="AAY154" s="0"/>
-      <c r="AAZ154" s="0"/>
-      <c r="ABA154" s="0"/>
-      <c r="ABB154" s="0"/>
-      <c r="ABC154" s="0"/>
-      <c r="ABD154" s="0"/>
-      <c r="ABE154" s="0"/>
-      <c r="ABF154" s="0"/>
-      <c r="ABG154" s="0"/>
-      <c r="ABH154" s="0"/>
-      <c r="ABI154" s="0"/>
-      <c r="ABJ154" s="0"/>
-      <c r="ABK154" s="0"/>
-      <c r="ABL154" s="0"/>
-      <c r="ABM154" s="0"/>
-      <c r="ABN154" s="0"/>
-      <c r="ABO154" s="0"/>
-      <c r="ABP154" s="0"/>
-      <c r="ABQ154" s="0"/>
-      <c r="ABR154" s="0"/>
-      <c r="ABS154" s="0"/>
-      <c r="ABT154" s="0"/>
-      <c r="ABU154" s="0"/>
-      <c r="ABV154" s="0"/>
-      <c r="ABW154" s="0"/>
-      <c r="ABX154" s="0"/>
-      <c r="ABY154" s="0"/>
-      <c r="ABZ154" s="0"/>
-      <c r="ACA154" s="0"/>
-      <c r="ACB154" s="0"/>
-      <c r="ACC154" s="0"/>
-      <c r="ACD154" s="0"/>
-      <c r="ACE154" s="0"/>
-      <c r="ACF154" s="0"/>
-      <c r="ACG154" s="0"/>
-      <c r="ACH154" s="0"/>
-      <c r="ACI154" s="0"/>
-      <c r="ACJ154" s="0"/>
-      <c r="ACK154" s="0"/>
-      <c r="ACL154" s="0"/>
-      <c r="ACM154" s="0"/>
-      <c r="ACN154" s="0"/>
-      <c r="ACO154" s="0"/>
-      <c r="ACP154" s="0"/>
-      <c r="ACQ154" s="0"/>
-      <c r="ACR154" s="0"/>
-      <c r="ACS154" s="0"/>
-      <c r="ACT154" s="0"/>
-      <c r="ACU154" s="0"/>
-      <c r="ACV154" s="0"/>
-      <c r="ACW154" s="0"/>
-      <c r="ACX154" s="0"/>
-      <c r="ACY154" s="0"/>
-      <c r="ACZ154" s="0"/>
-      <c r="ADA154" s="0"/>
-      <c r="ADB154" s="0"/>
-      <c r="ADC154" s="0"/>
-      <c r="ADD154" s="0"/>
-      <c r="ADE154" s="0"/>
-      <c r="ADF154" s="0"/>
-      <c r="ADG154" s="0"/>
-      <c r="ADH154" s="0"/>
-      <c r="ADI154" s="0"/>
-      <c r="ADJ154" s="0"/>
-      <c r="ADK154" s="0"/>
-      <c r="ADL154" s="0"/>
-      <c r="ADM154" s="0"/>
-      <c r="ADN154" s="0"/>
-      <c r="ADO154" s="0"/>
-      <c r="ADP154" s="0"/>
-      <c r="ADQ154" s="0"/>
-      <c r="ADR154" s="0"/>
-      <c r="ADS154" s="0"/>
-      <c r="ADT154" s="0"/>
-      <c r="ADU154" s="0"/>
-      <c r="ADV154" s="0"/>
-      <c r="ADW154" s="0"/>
-      <c r="ADX154" s="0"/>
-      <c r="ADY154" s="0"/>
-      <c r="ADZ154" s="0"/>
-      <c r="AEA154" s="0"/>
-      <c r="AEB154" s="0"/>
-      <c r="AEC154" s="0"/>
-      <c r="AED154" s="0"/>
-      <c r="AEE154" s="0"/>
-      <c r="AEF154" s="0"/>
-      <c r="AEG154" s="0"/>
-      <c r="AEH154" s="0"/>
-      <c r="AEI154" s="0"/>
-      <c r="AEJ154" s="0"/>
-      <c r="AEK154" s="0"/>
-      <c r="AEL154" s="0"/>
-      <c r="AEM154" s="0"/>
-      <c r="AEN154" s="0"/>
-      <c r="AEO154" s="0"/>
-      <c r="AEP154" s="0"/>
-      <c r="AEQ154" s="0"/>
-      <c r="AER154" s="0"/>
-      <c r="AES154" s="0"/>
-      <c r="AET154" s="0"/>
-      <c r="AEU154" s="0"/>
-      <c r="AEV154" s="0"/>
-      <c r="AEW154" s="0"/>
-      <c r="AEX154" s="0"/>
-      <c r="AEY154" s="0"/>
-      <c r="AEZ154" s="0"/>
-      <c r="AFA154" s="0"/>
-      <c r="AFB154" s="0"/>
-      <c r="AFC154" s="0"/>
-      <c r="AFD154" s="0"/>
-      <c r="AFE154" s="0"/>
-      <c r="AFF154" s="0"/>
-      <c r="AFG154" s="0"/>
-      <c r="AFH154" s="0"/>
-      <c r="AFI154" s="0"/>
-      <c r="AFJ154" s="0"/>
-      <c r="AFK154" s="0"/>
-      <c r="AFL154" s="0"/>
-      <c r="AFM154" s="0"/>
-      <c r="AFN154" s="0"/>
-      <c r="AFO154" s="0"/>
-      <c r="AFP154" s="0"/>
-      <c r="AFQ154" s="0"/>
-      <c r="AFR154" s="0"/>
-      <c r="AFS154" s="0"/>
-      <c r="AFT154" s="0"/>
-      <c r="AFU154" s="0"/>
-      <c r="AFV154" s="0"/>
-      <c r="AFW154" s="0"/>
-      <c r="AFX154" s="0"/>
-      <c r="AFY154" s="0"/>
-      <c r="AFZ154" s="0"/>
-      <c r="AGA154" s="0"/>
-      <c r="AGB154" s="0"/>
-      <c r="AGC154" s="0"/>
-      <c r="AGD154" s="0"/>
-      <c r="AGE154" s="0"/>
-      <c r="AGF154" s="0"/>
-      <c r="AGG154" s="0"/>
-      <c r="AGH154" s="0"/>
-      <c r="AGI154" s="0"/>
-      <c r="AGJ154" s="0"/>
-      <c r="AGK154" s="0"/>
-      <c r="AGL154" s="0"/>
-      <c r="AGM154" s="0"/>
-      <c r="AGN154" s="0"/>
-      <c r="AGO154" s="0"/>
-      <c r="AGP154" s="0"/>
-      <c r="AGQ154" s="0"/>
-      <c r="AGR154" s="0"/>
-      <c r="AGS154" s="0"/>
-      <c r="AGT154" s="0"/>
-      <c r="AGU154" s="0"/>
-      <c r="AGV154" s="0"/>
-      <c r="AGW154" s="0"/>
-      <c r="AGX154" s="0"/>
-      <c r="AGY154" s="0"/>
-      <c r="AGZ154" s="0"/>
-      <c r="AHA154" s="0"/>
-      <c r="AHB154" s="0"/>
-      <c r="AHC154" s="0"/>
-      <c r="AHD154" s="0"/>
-      <c r="AHE154" s="0"/>
-      <c r="AHF154" s="0"/>
-      <c r="AHG154" s="0"/>
-      <c r="AHH154" s="0"/>
-      <c r="AHI154" s="0"/>
-      <c r="AHJ154" s="0"/>
-      <c r="AHK154" s="0"/>
-      <c r="AHL154" s="0"/>
-      <c r="AHM154" s="0"/>
-      <c r="AHN154" s="0"/>
-      <c r="AHO154" s="0"/>
-      <c r="AHP154" s="0"/>
-      <c r="AHQ154" s="0"/>
-      <c r="AHR154" s="0"/>
-      <c r="AHS154" s="0"/>
-      <c r="AHT154" s="0"/>
-      <c r="AHU154" s="0"/>
-      <c r="AHV154" s="0"/>
-      <c r="AHW154" s="0"/>
-      <c r="AHX154" s="0"/>
-      <c r="AHY154" s="0"/>
-      <c r="AHZ154" s="0"/>
-      <c r="AIA154" s="0"/>
-      <c r="AIB154" s="0"/>
-      <c r="AIC154" s="0"/>
-      <c r="AID154" s="0"/>
-      <c r="AIE154" s="0"/>
-      <c r="AIF154" s="0"/>
-      <c r="AIG154" s="0"/>
-      <c r="AIH154" s="0"/>
-      <c r="AII154" s="0"/>
-      <c r="AIJ154" s="0"/>
-      <c r="AIK154" s="0"/>
-      <c r="AIL154" s="0"/>
-      <c r="AIM154" s="0"/>
-      <c r="AIN154" s="0"/>
-      <c r="AIO154" s="0"/>
-      <c r="AIP154" s="0"/>
-      <c r="AIQ154" s="0"/>
-      <c r="AIR154" s="0"/>
-      <c r="AIS154" s="0"/>
-      <c r="AIT154" s="0"/>
-      <c r="AIU154" s="0"/>
-      <c r="AIV154" s="0"/>
-      <c r="AIW154" s="0"/>
-      <c r="AIX154" s="0"/>
-      <c r="AIY154" s="0"/>
-      <c r="AIZ154" s="0"/>
-      <c r="AJA154" s="0"/>
-      <c r="AJB154" s="0"/>
-      <c r="AJC154" s="0"/>
-      <c r="AJD154" s="0"/>
-      <c r="AJE154" s="0"/>
-      <c r="AJF154" s="0"/>
-      <c r="AJG154" s="0"/>
-      <c r="AJH154" s="0"/>
-      <c r="AJI154" s="0"/>
-      <c r="AJJ154" s="0"/>
-      <c r="AJK154" s="0"/>
-      <c r="AJL154" s="0"/>
-      <c r="AJM154" s="0"/>
-      <c r="AJN154" s="0"/>
-      <c r="AJO154" s="0"/>
-      <c r="AJP154" s="0"/>
-      <c r="AJQ154" s="0"/>
-      <c r="AJR154" s="0"/>
-      <c r="AJS154" s="0"/>
-      <c r="AJT154" s="0"/>
-      <c r="AJU154" s="0"/>
-      <c r="AJV154" s="0"/>
-      <c r="AJW154" s="0"/>
-      <c r="AJX154" s="0"/>
-      <c r="AJY154" s="0"/>
-      <c r="AJZ154" s="0"/>
-      <c r="AKA154" s="0"/>
-      <c r="AKB154" s="0"/>
-      <c r="AKC154" s="0"/>
-      <c r="AKD154" s="0"/>
-      <c r="AKE154" s="0"/>
-      <c r="AKF154" s="0"/>
-      <c r="AKG154" s="0"/>
-      <c r="AKH154" s="0"/>
-      <c r="AKI154" s="0"/>
-      <c r="AKJ154" s="0"/>
-      <c r="AKK154" s="0"/>
-      <c r="AKL154" s="0"/>
-      <c r="AKM154" s="0"/>
-      <c r="AKN154" s="0"/>
-      <c r="AKO154" s="0"/>
-      <c r="AKP154" s="0"/>
-      <c r="AKQ154" s="0"/>
-      <c r="AKR154" s="0"/>
-      <c r="AKS154" s="0"/>
-      <c r="AKT154" s="0"/>
-      <c r="AKU154" s="0"/>
-      <c r="AKV154" s="0"/>
-      <c r="AKW154" s="0"/>
-      <c r="AKX154" s="0"/>
-      <c r="AKY154" s="0"/>
-      <c r="AKZ154" s="0"/>
-      <c r="ALA154" s="0"/>
-      <c r="ALB154" s="0"/>
-      <c r="ALC154" s="0"/>
-      <c r="ALD154" s="0"/>
-      <c r="ALE154" s="0"/>
-      <c r="ALF154" s="0"/>
-      <c r="ALG154" s="0"/>
-      <c r="ALH154" s="0"/>
-      <c r="ALI154" s="0"/>
-      <c r="ALJ154" s="0"/>
-      <c r="ALK154" s="0"/>
-      <c r="ALL154" s="0"/>
-      <c r="ALM154" s="0"/>
-      <c r="ALN154" s="0"/>
-      <c r="ALO154" s="0"/>
-      <c r="ALP154" s="0"/>
-      <c r="ALQ154" s="0"/>
-      <c r="ALR154" s="0"/>
-      <c r="ALS154" s="0"/>
-      <c r="ALT154" s="0"/>
-      <c r="ALU154" s="0"/>
-      <c r="ALV154" s="0"/>
-      <c r="ALW154" s="0"/>
-      <c r="ALX154" s="0"/>
-      <c r="ALY154" s="0"/>
-      <c r="ALZ154" s="0"/>
-      <c r="AMA154" s="0"/>
-      <c r="AMB154" s="0"/>
-      <c r="AMC154" s="0"/>
-      <c r="AMD154" s="0"/>
-      <c r="AME154" s="0"/>
-      <c r="AMF154" s="0"/>
-      <c r="AMG154" s="0"/>
-      <c r="AMH154" s="0"/>
-      <c r="AMI154" s="0"/>
-      <c r="AMJ154" s="0"/>
+      <c r="H154" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K154" s="5" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="155" s="3" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="2"/>
     </row>
     <row r="156" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F156" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G156" s="3" t="n">
         <f aca="false">SUM(G1:G154)</f>

</xml_diff>

<commit_message>
More updates to step 3 and started work on Bom
</commit_message>
<xml_diff>
--- a/notes/My_BoM.xlsx
+++ b/notes/My_BoM.xlsx
@@ -76,25 +76,7 @@
     <t xml:space="preserve">FYSETC (Aliexp)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">"Full Set Kit". </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">This isn’t actually the one I ordered but I believe it’s the same kit. Mine isn’t available any longer</t>
-    </r>
+    <t xml:space="preserve">"Full Set Kit". This isn’t actually the one I ordered but I believe it’s the same kit. Mine isn’t available any longer</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.aliexpress.com/item/33048238537.html?spm=a2g0o.productlist.0.0.3b59553bEb0n4Z&amp;algo_pvid=ee9d284c-5474-4a38-9f09-9532647a402f&amp;algo_expid=ee9d284c-5474-4a38-9f09-9532647a402f-2&amp;btsid=0b0a556216108909047922816e4e3b&amp;ws_ab_test=searchweb0_0,searchweb201602_,searchweb201603_</t>
@@ -596,7 +578,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -642,12 +624,6 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -691,7 +667,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -705,10 +681,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -736,10 +708,10 @@
   <dimension ref="A2:L158"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.48"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="1" width="14.43"/>
@@ -849,7 +821,7 @@
       <c r="I7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K7" s="1" t="s">
@@ -2705,32 +2677,32 @@
         <v>11</v>
       </c>
     </row>
-    <row r="154" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="5" t="s">
+    <row r="154" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="B154" s="5" t="s">
+      <c r="B154" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C154" s="5" t="n">
+      <c r="C154" s="4" t="n">
         <v>3.04</v>
       </c>
-      <c r="D154" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E154" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F154" s="5" t="n">
+      <c r="D154" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E154" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F154" s="4" t="n">
         <v>3.04</v>
       </c>
-      <c r="G154" s="5" t="n">
+      <c r="G154" s="4" t="n">
         <v>3.04</v>
       </c>
-      <c r="H154" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K154" s="5" t="s">
+      <c r="H154" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K154" s="4" t="s">
         <v>181</v>
       </c>
     </row>

</xml_diff>